<commit_message>
inclusao dos valores de tensao maxima no excel
</commit_message>
<xml_diff>
--- a/medicoes.xlsx
+++ b/medicoes.xlsx
@@ -1,21 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeronimo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeronimo/Desktop/eletromag/projeto_2022_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F74FD68B-097F-8745-A497-F00A78EA41F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBA2431-A06F-244B-9320-02D8C6A8FECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{911F66AB-CAA0-FC46-8627-F248D8A0855E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{911F66AB-CAA0-FC46-8627-F248D8A0855E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Planilha1!$A$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Planilha1!$A$2:$A$9</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Planilha1!$B$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Planilha1!$B$2:$B$9</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Planilha1!$C$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Planilha1!$C$2:$C$9</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">Planilha1!$C$1</definedName>
+    <definedName name="_xlchart.v2.11" hidden="1">Planilha1!$C$2:$C$9</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">Planilha1!$A$1</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">Planilha1!$A$2:$A$9</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">Planilha1!$B$1</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">Planilha1!$B$2:$B$9</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +37,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Distância (cm)</t>
   </si>
@@ -63,14 +83,24 @@
   </si>
   <si>
     <t>6,2 cm</t>
+  </si>
+  <si>
+    <t>Watts</t>
+  </si>
+  <si>
+    <t>V RMS</t>
+  </si>
+  <si>
+    <t>V pico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -101,9 +131,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D5F98D-F7FE-9E47-B4A7-A555D81874D0}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,7 +588,7 @@
         <v>0.41250000000000003</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
+        <f>C5*C5/$H$3</f>
         <v>0.1764</v>
       </c>
       <c r="F5" s="1">
@@ -663,6 +694,30 @@
       </c>
       <c r="B11" t="s">
         <v>10</v>
+      </c>
+      <c r="C11">
+        <v>7.3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="2">
+        <f xml:space="preserve"> C11 / SQRT(2)</f>
+        <v>5.1618795026617965</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="2">
+        <f>C12*C12/H3</f>
+        <v>0.26644999999999996</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inclusão do preço dos componentes no excel
</commit_message>
<xml_diff>
--- a/medicoes.xlsx
+++ b/medicoes.xlsx
@@ -8,27 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeronimo/Desktop/eletromag/projeto_2022_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBA2431-A06F-244B-9320-02D8C6A8FECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A039662-51DA-C24F-A622-38BC2FE74E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{911F66AB-CAA0-FC46-8627-F248D8A0855E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{911F66AB-CAA0-FC46-8627-F248D8A0855E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="medicoes" sheetId="1" r:id="rId1"/>
+    <sheet name="preco_componentes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Planilha1!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Planilha1!$A$2:$A$9</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Planilha1!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Planilha1!$B$2:$B$9</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Planilha1!$C$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Planilha1!$C$2:$C$9</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">Planilha1!$C$1</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">Planilha1!$C$2:$C$9</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">Planilha1!$A$1</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">Planilha1!$A$2:$A$9</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">Planilha1!$B$1</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">Planilha1!$B$2:$B$9</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -50,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Distância (cm)</t>
   </si>
@@ -92,18 +79,85 @@
   </si>
   <si>
     <t>V pico</t>
+  </si>
+  <si>
+    <t>Componente</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Preco Unit</t>
+  </si>
+  <si>
+    <t>Preco total</t>
+  </si>
+  <si>
+    <t>0.1uF 1kVDC film capacitor X1 rated</t>
+  </si>
+  <si>
+    <t>N channel MOSFET</t>
+  </si>
+  <si>
+    <t>8-DIP half bridge driver IC</t>
+  </si>
+  <si>
+    <t>0.1uF ceramic capacitor</t>
+  </si>
+  <si>
+    <t>470uF 16v aluminum electrolytic capacitor</t>
+  </si>
+  <si>
+    <t>Bobina Receptor</t>
+  </si>
+  <si>
+    <t>Bobina Transmissor</t>
+  </si>
+  <si>
+    <t>Resistor 1k</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>40V schottky diode</t>
+  </si>
+  <si>
+    <t>POTÊNCIA REAL MEDIDA (W)</t>
+  </si>
+  <si>
+    <t>POTÊNCIA REAL POR CUSTO (W/R$)</t>
+  </si>
+  <si>
+    <t>CUSTO POR POTÊNCIA REAL (R$/W)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -128,15 +182,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D5F98D-F7FE-9E47-B4A7-A555D81874D0}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -723,4 +784,214 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF326033-9DFD-AC4C-A133-65DFD10D5083}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>7.28</v>
+      </c>
+      <c r="D2" s="3">
+        <f>C2*B2</f>
+        <v>14.56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>6.0020999999999995</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D10" si="0">C3*B3</f>
+        <v>12.004199999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>28.163700000000002</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>28.163700000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>0.20602000000000001</v>
+      </c>
+      <c r="C7" s="3">
+        <v>133</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>27.400660000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>0.20347999999999999</v>
+      </c>
+      <c r="C8" s="3">
+        <v>133</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>27.062839999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="5">
+        <f>SUM(D2:D10)</f>
+        <v>115.05140000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="7">
+        <f>medicoes!C13</f>
+        <v>0.26644999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="6">
+        <f>D13/D12</f>
+        <v>2.3159214055630782E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="5">
+        <f>1/D14</f>
+        <v>431.79358228560716</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>